<commit_message>
Ran NasNetMobile and saved the results. Added another notebook for fine tuning.
</commit_message>
<xml_diff>
--- a/LATEST_RESULTS/Results.xlsx
+++ b/LATEST_RESULTS/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Model</t>
   </si>
@@ -33,9 +33,6 @@
     <t>AUC</t>
   </si>
   <si>
-    <t>Recall (0.3)</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -45,34 +42,88 @@
     <t>mobilenet</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>Epochs</t>
-  </si>
-  <si>
     <t>Tlearn</t>
   </si>
   <si>
     <t>Cweights</t>
   </si>
   <si>
-    <t>BCE</t>
-  </si>
-  <si>
-    <t>Resolution</t>
-  </si>
-  <si>
-    <t>Batch Size</t>
+    <t>k</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>bce</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>nasnetmobile</t>
+  </si>
+  <si>
+    <t>Prec</t>
+  </si>
+  <si>
+    <t>Edema</t>
+  </si>
+  <si>
+    <t>Fibrosis</t>
+  </si>
+  <si>
+    <t>Hernia</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Nodule</t>
+  </si>
+  <si>
+    <t>Atelect</t>
+  </si>
+  <si>
+    <t>Cardiomeg</t>
+  </si>
+  <si>
+    <t>Consolida</t>
+  </si>
+  <si>
+    <t>Effuss</t>
+  </si>
+  <si>
+    <t>Emphys</t>
+  </si>
+  <si>
+    <t>Infiltra</t>
+  </si>
+  <si>
+    <t>No Fin</t>
+  </si>
+  <si>
+    <t>Pleu_Thick</t>
+  </si>
+  <si>
+    <t>Pneumo</t>
+  </si>
+  <si>
+    <t>Pne_thorax</t>
+  </si>
+  <si>
+    <t>Resol</t>
+  </si>
+  <si>
+    <t>Epo</t>
+  </si>
+  <si>
+    <t>BSize</t>
+  </si>
+  <si>
+    <t>Reca (0.3)</t>
   </si>
 </sst>
 </file>
@@ -404,29 +455,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O53"/>
+  <dimension ref="A1:AD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="1.33203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -437,43 +505,90 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1">
         <v>9.6999999999999993</v>
@@ -488,13 +603,13 @@
         <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L2" s="1">
         <v>80</v>
@@ -507,15 +622,15 @@
       </c>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>5.2</v>
@@ -530,13 +645,13 @@
         <v>16</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L3" s="1">
         <v>81</v>
@@ -549,67 +664,216 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1">
+        <v>300</v>
+      </c>
+      <c r="H4" s="1">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="1">
+        <v>80</v>
+      </c>
+      <c r="M4" s="1">
+        <v>56.1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>54.7</v>
+      </c>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>400</v>
+      </c>
+      <c r="H5" s="1">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="1">
+        <v>80</v>
+      </c>
+      <c r="M5" s="1">
+        <v>56.7</v>
+      </c>
+      <c r="N5" s="1">
+        <v>55.5</v>
+      </c>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>500</v>
+      </c>
+      <c r="H6" s="1">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>224</v>
+      </c>
+      <c r="H7" s="1">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="1">
+        <v>79</v>
+      </c>
+      <c r="M7" s="1">
+        <v>52.5</v>
+      </c>
+      <c r="N7" s="1">
+        <v>54.3</v>
+      </c>
+      <c r="O7" s="1">
+        <v>56.2</v>
+      </c>
+      <c r="P7" s="1">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>82</v>
+      </c>
+      <c r="R7" s="1">
+        <v>77</v>
+      </c>
+      <c r="S7" s="1">
+        <v>82</v>
+      </c>
+      <c r="T7" s="1">
+        <v>77</v>
+      </c>
+      <c r="U7" s="1">
+        <v>73</v>
+      </c>
+      <c r="V7" s="1">
+        <v>79</v>
+      </c>
+      <c r="W7" s="1">
+        <v>87</v>
+      </c>
+      <c r="X7" s="1">
+        <v>72</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>75</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>80</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>88</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>86</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>88</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -624,7 +888,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -639,7 +903,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -654,7 +918,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -669,7 +933,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -684,7 +948,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -699,7 +963,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -714,7 +978,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -729,7 +993,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1299,6 +1563,21 @@
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
     </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>